<commit_message>
added updated bar chart
</commit_message>
<xml_diff>
--- a/data/DengueCases2023.xlsx
+++ b/data/DengueCases2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\01 Projects\Dashboards\dengue-situation-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27097CA4-D2B8-40A4-ACCC-68D9B993F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164E6268-290F-4353-944C-93102E85FA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35306,7 +35306,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>